<commit_message>
Function for reading an Excel file and set-up for cronjob
</commit_message>
<xml_diff>
--- a/app/files/2021-StMM-Overzicht-Weezenkerkhof.xlsx
+++ b/app/files/2021-StMM-Overzicht-Weezenkerkhof.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\SSS-dev\webapplication-stichting-memento-mori\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAF443AF-F19C-4B9D-A967-46EC3E348045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35E865-8412-4056-B825-B0B30C797A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CC40A5F-39CE-A24E-BAE0-2D8E0A6EA817}"/>
   </bookViews>
@@ -34,36 +34,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="489">
   <si>
-    <t>Achternaam </t>
-  </si>
-  <si>
-    <t>Tussenv.</t>
-  </si>
-  <si>
-    <t>Voorna(a)m(en)</t>
-  </si>
-  <si>
     <t>Periode</t>
   </si>
   <si>
-    <t>Geb.datum </t>
-  </si>
-  <si>
-    <t>Geboorteplaats </t>
-  </si>
-  <si>
     <t>Leeftijd</t>
   </si>
   <si>
     <t>Overlijden </t>
   </si>
   <si>
-    <t>Reden overl.</t>
-  </si>
-  <si>
-    <t>Begraven </t>
-  </si>
-  <si>
     <t>Soort graf</t>
   </si>
   <si>
@@ -787,9 +766,6 @@
     <t>(1937-1938)</t>
   </si>
   <si>
-    <t xml:space="preserve">36a  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Kruijf </t>
   </si>
   <si>
@@ -1465,9 +1441,6 @@
     <t>Huisvrouw, moeder en weezenvriend</t>
   </si>
   <si>
-    <t>Grafnr.</t>
-  </si>
-  <si>
     <t>Hendrik</t>
   </si>
   <si>
@@ -1499,6 +1472,33 @@
   </si>
   <si>
     <t>Uitstrooing as:  Oud Weezendag 2021</t>
+  </si>
+  <si>
+    <t>36a</t>
+  </si>
+  <si>
+    <t>Achternaam</t>
+  </si>
+  <si>
+    <t>Geboorteplaats</t>
+  </si>
+  <si>
+    <t>Begraven</t>
+  </si>
+  <si>
+    <t>Grafnummer</t>
+  </si>
+  <si>
+    <t>Tussenvoegsel</t>
+  </si>
+  <si>
+    <t>Voornamen</t>
+  </si>
+  <si>
+    <t>Geboortedatum</t>
+  </si>
+  <si>
+    <t>Reden overlijden</t>
   </si>
 </sst>
 </file>
@@ -2449,9 +2449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC831DE1-BD87-6B4F-B4E8-1B2FF245A412}">
   <dimension ref="A1:T438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2479,63 +2479,63 @@
     <col min="21" max="16384" width="33.5" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="R1" s="116" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="S1" s="117" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="T1" s="120"/>
     </row>
@@ -2544,126 +2544,126 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="7"/>
       <c r="N2" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="R2" s="13"/>
       <c r="S2" s="118"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G3" s="15">
         <v>5410</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I3" s="100" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J3" s="16">
         <v>79</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R3" s="13"/>
       <c r="S3" s="118"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G4" s="83">
         <v>1559</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="I4" s="101" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="J4" s="18">
         <v>90</v>
@@ -2676,46 +2676,46 @@
         <v>34520</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="R4" s="13"/>
       <c r="S4" s="118"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I5" s="100" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K5" s="84">
         <v>30709</v>
@@ -2725,43 +2725,43 @@
         <v>30713</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="R5" s="13"/>
       <c r="S5" s="118"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I6" s="100" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J6" s="19">
         <v>99</v>
@@ -2770,53 +2770,53 @@
         <v>42659</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="M6" s="84">
         <v>42667</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="118" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G7" s="112">
         <v>19227</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="I7" s="102" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J7" s="24">
         <v>58</v>
@@ -2825,26 +2825,26 @@
         <v>40612</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="O7" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="118" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2852,26 +2852,26 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G8" s="76" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I8" s="100" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="J8" s="19">
         <v>78</v>
@@ -2880,20 +2880,20 @@
         <v>30710</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="R8" s="13"/>
       <c r="S8" s="118"/>
@@ -2903,28 +2903,28 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G9" s="77">
         <v>7086</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I9" s="100" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J9" s="19">
         <v>64</v>
@@ -2935,16 +2935,16 @@
       <c r="L9" s="8"/>
       <c r="M9" s="7"/>
       <c r="N9" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="R9" s="13"/>
       <c r="S9" s="118"/>
@@ -2954,26 +2954,26 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G10" s="77">
         <v>13257</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I10" s="100" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J10" s="19">
         <v>43</v>
@@ -2982,51 +2982,51 @@
         <v>29490</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="M10" s="84">
         <v>29495</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="118"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G11" s="77">
         <v>2975</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I11" s="100" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="J11" s="19">
         <v>69</v>
@@ -3035,53 +3035,53 @@
         <v>28347</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="M11" s="84">
         <v>28352</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R11" s="111"/>
       <c r="S11" s="118"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G12" s="77">
         <v>897</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I12" s="100" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J12" s="19">
         <v>76</v>
@@ -3090,49 +3090,49 @@
         <v>29015</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="M12" s="84">
         <v>28989</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="R12" s="111"/>
       <c r="S12" s="118"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G13" s="77">
         <v>716</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I13" s="100" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J13" s="19">
         <v>74</v>
@@ -3145,43 +3145,43 @@
         <v>27575</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="R13" s="111"/>
       <c r="S13" s="118"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G14" s="77">
         <v>4022</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="I14" s="100" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="J14" s="19">
         <v>62</v>
@@ -3194,43 +3194,43 @@
         <v>26997</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="R14" s="13"/>
       <c r="S14" s="118"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G15" s="77">
         <v>4537</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I15" s="100" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="J15" s="19">
         <v>63</v>
@@ -3243,43 +3243,43 @@
         <v>28003</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="118"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G16" s="77">
         <v>890</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I16" s="100" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J16" s="19">
         <v>71</v>
@@ -3292,47 +3292,47 @@
         <v>26856</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="R16" s="13"/>
       <c r="S16" s="118"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G17" s="77">
         <v>4672</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I17" s="100" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J17" s="19">
         <v>55</v>
@@ -3345,43 +3345,43 @@
         <v>24705</v>
       </c>
       <c r="N17" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="R17" s="13"/>
       <c r="S17" s="118"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G18" s="77">
         <v>6187</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I18" s="100" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J18" s="19">
         <v>67</v>
@@ -3394,47 +3394,47 @@
         <v>30669</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R18" s="13"/>
       <c r="S18" s="118"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G19" s="112">
         <v>17576</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I19" s="102" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J19" s="24">
         <v>53</v>
@@ -3445,43 +3445,43 @@
       <c r="L19" s="22"/>
       <c r="M19" s="21"/>
       <c r="N19" s="23" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="O19" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P19" s="22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q19" s="22" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="R19" s="13"/>
       <c r="S19" s="118"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="27" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="28" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G20" s="123">
         <v>14140</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I20" s="103" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="J20" s="31">
         <v>14</v>
@@ -3490,53 +3490,53 @@
         <v>19371</v>
       </c>
       <c r="L20" s="28" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="M20" s="124">
         <v>19374</v>
       </c>
       <c r="N20" s="29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O20" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P20" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="R20" s="13"/>
       <c r="S20" s="118" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G21" s="77">
         <v>1391</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I21" s="100" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J21" s="19">
         <v>54</v>
@@ -3549,45 +3549,45 @@
         <v>20999</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="R21" s="93" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="S21" s="118"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G22" s="77">
         <v>8033</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I22" s="100" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J22" s="19">
         <v>37</v>
@@ -3596,51 +3596,51 @@
         <v>21911</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="M22" s="84">
         <v>21915</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q22" s="8" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="R22" s="13"/>
       <c r="S22" s="118"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B23" s="88" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C23" s="88" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D23" s="88" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E23" s="88"/>
       <c r="F23" s="60" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G23" s="114">
         <v>13397</v>
       </c>
       <c r="H23" s="89" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I23" s="104" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J23" s="90">
         <v>81</v>
@@ -3649,51 +3649,51 @@
         <v>6597</v>
       </c>
       <c r="L23" s="60" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="M23" s="115">
         <v>6601</v>
       </c>
       <c r="N23" s="91" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O23" s="60" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="P23" s="60" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q23" s="60" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="R23" s="13"/>
       <c r="S23" s="118" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="68" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B24" s="88" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="88" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E24" s="88"/>
       <c r="F24" s="60" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G24" s="125" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="H24" s="89" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I24" s="104" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J24" s="90">
         <v>63</v>
@@ -3704,20 +3704,20 @@
       <c r="L24" s="60"/>
       <c r="M24" s="88"/>
       <c r="N24" s="91" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O24" s="60" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="P24" s="60" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q24" s="60" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="R24" s="13"/>
       <c r="S24" s="118" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -3725,24 +3725,24 @@
         <v>17</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G25" s="76" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I25" s="101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J25" s="19">
         <v>79</v>
@@ -3755,45 +3755,45 @@
         <v>2851</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="R25" s="13"/>
       <c r="S25" s="118"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G26" s="76" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I26" s="101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J26" s="19">
         <v>51</v>
@@ -3802,49 +3802,49 @@
         <v>2749</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="M26" s="84">
         <v>2753</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q26" s="8" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="R26" s="13"/>
       <c r="S26" s="118"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G27" s="76" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="I27" s="101" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J27" s="19">
         <v>74</v>
@@ -3857,92 +3857,92 @@
         <v>9359</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="R27" s="13"/>
       <c r="S27" s="118"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="E28" s="33"/>
       <c r="F28" s="34" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G28" s="79" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I28" s="105" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J28" s="36">
         <v>55</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="L28" s="34" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="M28" s="33"/>
       <c r="N28" s="35" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O28" s="34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q28" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="R28" s="13"/>
       <c r="S28" s="118"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="33" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="E29" s="33"/>
       <c r="F29" s="34" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G29" s="79" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I29" s="105" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J29" s="36">
         <v>68</v>
@@ -3951,73 +3951,73 @@
         <v>897</v>
       </c>
       <c r="L29" s="34" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="M29" s="33"/>
       <c r="N29" s="35" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O29" s="34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="P29" s="34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q29" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="R29" s="13"/>
       <c r="S29" s="118"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G30" s="76" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I30" s="101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J30" s="19">
         <v>90</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q30" s="8" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="R30" s="13"/>
       <c r="S30" s="118" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -4025,124 +4025,124 @@
         <v>21</v>
       </c>
       <c r="B31" s="94" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C31" s="94"/>
       <c r="D31" s="94" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E31" s="94"/>
       <c r="F31" s="95" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G31" s="96" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="H31" s="95" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="I31" s="106" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="J31" s="97">
         <v>44</v>
       </c>
       <c r="K31" s="94" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="L31" s="95" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="M31" s="94"/>
       <c r="N31" s="98" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O31" s="95" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P31" s="95" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q31" s="95" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="R31" s="93" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="S31" s="118"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G32" s="76" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="I32" s="101" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J32" s="19">
         <v>52</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q32" s="8" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="R32" s="13"/>
       <c r="S32" s="118"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G33" s="76" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I33" s="101" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J33" s="19">
         <v>51</v>
@@ -4151,51 +4151,51 @@
         <v>7768</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="M33" s="84">
         <v>7772</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="R33" s="13"/>
       <c r="S33" s="118"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G34" s="76" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="I34" s="101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J34" s="19">
         <v>80</v>
@@ -4208,16 +4208,16 @@
         <v>18013</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q34" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R34" s="13"/>
       <c r="S34" s="118"/>
@@ -4227,24 +4227,24 @@
         <v>24</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G35" s="76" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="I35" s="101" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J35" s="19">
         <v>59</v>
@@ -4253,49 +4253,49 @@
         <v>8087</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="M35" s="84">
         <v>8091</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="R35" s="13"/>
       <c r="S35" s="118"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G36" s="76" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I36" s="101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="J36" s="19">
         <v>50</v>
@@ -4308,43 +4308,43 @@
         <v>9299</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q36" s="8" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="R36" s="13"/>
       <c r="S36" s="118"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G37" s="76" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I37" s="101" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J37" s="19">
         <v>63</v>
@@ -4353,49 +4353,49 @@
         <v>13223</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="M37" s="84">
         <v>13227</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O37" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q37" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="R37" s="13"/>
       <c r="S37" s="118"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="22" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G38" s="112">
         <v>3444</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="I38" s="102" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J38" s="24">
         <v>41</v>
@@ -4408,43 +4408,43 @@
         <v>18777</v>
       </c>
       <c r="N38" s="23" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O38" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q38" s="22" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="R38" s="13"/>
       <c r="S38" s="118"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="8" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G39" s="76" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="I39" s="101" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J39" s="19">
         <v>89</v>
@@ -4457,43 +4457,43 @@
         <v>23614</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q39" s="8" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="R39" s="13"/>
       <c r="S39" s="118"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G40" s="76" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="I40" s="101" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J40" s="19">
         <v>47</v>
@@ -4502,49 +4502,49 @@
         <v>16585</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="M40" s="84">
         <v>16588</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="R40" s="13"/>
       <c r="S40" s="118"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G41" s="76" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="I41" s="101" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="J41" s="19">
         <v>58</v>
@@ -4553,22 +4553,22 @@
         <v>18386</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="M41" s="84">
         <v>18389</v>
       </c>
       <c r="N41" s="25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O41" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q41" s="8" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="R41" s="13"/>
       <c r="S41" s="118"/>
@@ -4578,26 +4578,26 @@
         <v>29</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="28" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G42" s="123">
         <v>13546</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="I42" s="107" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J42" s="31">
         <v>10</v>
@@ -4606,44 +4606,44 @@
         <v>17351</v>
       </c>
       <c r="L42" s="28" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="M42" s="124">
         <v>17355</v>
       </c>
       <c r="N42" s="29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O42" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P42" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="R42" s="13"/>
       <c r="S42" s="118" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G43" s="78"/>
       <c r="H43" s="28"/>
@@ -4653,13 +4653,13 @@
       <c r="L43" s="28"/>
       <c r="M43" s="27"/>
       <c r="N43" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O43" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P43" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q43" s="28"/>
       <c r="R43" s="13"/>
@@ -4667,38 +4667,38 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="27" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G44" s="78"/>
       <c r="H44" s="28"/>
       <c r="I44" s="107"/>
       <c r="J44" s="31" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="K44" s="27"/>
       <c r="L44" s="28"/>
       <c r="M44" s="27"/>
       <c r="N44" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O44" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P44" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q44" s="28"/>
       <c r="R44" s="13"/>
@@ -4706,20 +4706,20 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="27" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G45" s="78"/>
       <c r="H45" s="28"/>
@@ -4729,42 +4729,42 @@
       </c>
       <c r="K45" s="27"/>
       <c r="L45" s="28" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="M45" s="27"/>
       <c r="N45" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O45" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P45" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q45" s="28" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="R45" s="13"/>
       <c r="S45" s="118"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="38" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="F46" s="40" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="G46" s="80"/>
       <c r="H46" s="40"/>
@@ -4774,13 +4774,13 @@
       <c r="L46" s="40"/>
       <c r="M46" s="39"/>
       <c r="N46" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O46" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P46" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q46" s="40"/>
       <c r="R46" s="13"/>
@@ -4788,20 +4788,20 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="38" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C47" s="39"/>
       <c r="D47" s="39" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E47" s="39" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F47" s="40" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G47" s="80"/>
       <c r="H47" s="40"/>
@@ -4811,13 +4811,13 @@
       <c r="L47" s="40"/>
       <c r="M47" s="39"/>
       <c r="N47" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O47" s="40" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="P47" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q47" s="40"/>
       <c r="R47" s="13"/>
@@ -4825,18 +4825,18 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="28" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G48" s="78"/>
       <c r="H48" s="28"/>
@@ -4846,13 +4846,13 @@
       <c r="L48" s="28"/>
       <c r="M48" s="27"/>
       <c r="N48" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O48" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P48" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q48" s="28"/>
       <c r="R48" s="13"/>
@@ -4860,20 +4860,20 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G49" s="78"/>
       <c r="H49" s="28"/>
@@ -4883,13 +4883,13 @@
       <c r="L49" s="28"/>
       <c r="M49" s="27"/>
       <c r="N49" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O49" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q49" s="28"/>
       <c r="R49" s="13"/>
@@ -4897,20 +4897,20 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="38" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C50" s="39"/>
       <c r="D50" s="39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F50" s="40" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="G50" s="80"/>
       <c r="H50" s="40"/>
@@ -4920,13 +4920,13 @@
       <c r="L50" s="40"/>
       <c r="M50" s="39"/>
       <c r="N50" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O50" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P50" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q50" s="40"/>
       <c r="R50" s="13"/>
@@ -4934,18 +4934,18 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C51" s="39"/>
       <c r="D51" s="39" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E51" s="39"/>
       <c r="F51" s="40" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="G51" s="80"/>
       <c r="H51" s="40"/>
@@ -4955,13 +4955,13 @@
       <c r="L51" s="40"/>
       <c r="M51" s="39"/>
       <c r="N51" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O51" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P51" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q51" s="40"/>
       <c r="R51" s="13"/>
@@ -4969,20 +4969,20 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C52" s="27"/>
       <c r="D52" s="27" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G52" s="78"/>
       <c r="H52" s="28"/>
@@ -4992,13 +4992,13 @@
       <c r="L52" s="28"/>
       <c r="M52" s="27"/>
       <c r="N52" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O52" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P52" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q52" s="28"/>
       <c r="R52" s="13"/>
@@ -5006,18 +5006,18 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="38" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C53" s="39"/>
       <c r="D53" s="39" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="E53" s="39"/>
       <c r="F53" s="40" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G53" s="80"/>
       <c r="H53" s="40"/>
@@ -5027,13 +5027,13 @@
       <c r="L53" s="40"/>
       <c r="M53" s="39"/>
       <c r="N53" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O53" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P53" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q53" s="40"/>
       <c r="R53" s="13"/>
@@ -5041,20 +5041,20 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="38" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C54" s="39"/>
       <c r="D54" s="39" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="F54" s="40" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G54" s="80"/>
       <c r="H54" s="40"/>
@@ -5064,13 +5064,13 @@
       <c r="L54" s="40"/>
       <c r="M54" s="39"/>
       <c r="N54" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O54" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P54" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q54" s="40"/>
       <c r="R54" s="13"/>
@@ -5078,20 +5078,20 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="G55" s="75"/>
       <c r="H55" s="22"/>
@@ -5101,34 +5101,34 @@
       <c r="L55" s="22"/>
       <c r="M55" s="21"/>
       <c r="N55" s="29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O55" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P55" s="22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q55" s="22" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="R55" s="13"/>
       <c r="S55" s="118"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="27" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="28" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="G56" s="78"/>
       <c r="H56" s="28"/>
@@ -5138,13 +5138,13 @@
       <c r="L56" s="28"/>
       <c r="M56" s="27"/>
       <c r="N56" s="29" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O56" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P56" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q56" s="28"/>
       <c r="R56" s="13"/>
@@ -5152,18 +5152,18 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="38" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C57" s="39"/>
       <c r="D57" s="39" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E57" s="39"/>
       <c r="F57" s="40" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="G57" s="80"/>
       <c r="H57" s="40"/>
@@ -5173,13 +5173,13 @@
       <c r="L57" s="40"/>
       <c r="M57" s="39"/>
       <c r="N57" s="29" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O57" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P57" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q57" s="40"/>
       <c r="R57" s="13"/>
@@ -5187,20 +5187,20 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
-        <v>251</v>
+        <v>480</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="28" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G58" s="78"/>
       <c r="H58" s="28"/>
@@ -5210,13 +5210,13 @@
       <c r="L58" s="28"/>
       <c r="M58" s="27"/>
       <c r="N58" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O58" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P58" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q58" s="28"/>
       <c r="R58" s="13"/>
@@ -5224,18 +5224,18 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="38" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C59" s="39"/>
       <c r="D59" s="39" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E59" s="39"/>
       <c r="F59" s="40" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G59" s="80"/>
       <c r="H59" s="40"/>
@@ -5245,13 +5245,13 @@
       <c r="L59" s="40"/>
       <c r="M59" s="39"/>
       <c r="N59" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O59" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P59" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q59" s="40"/>
       <c r="R59" s="13"/>
@@ -5259,18 +5259,18 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="38" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C60" s="39"/>
       <c r="D60" s="39" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E60" s="39"/>
       <c r="F60" s="40" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G60" s="80"/>
       <c r="H60" s="40"/>
@@ -5280,13 +5280,13 @@
       <c r="L60" s="40"/>
       <c r="M60" s="39"/>
       <c r="N60" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O60" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P60" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q60" s="40"/>
       <c r="R60" s="13"/>
@@ -5294,18 +5294,18 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C61" s="27"/>
       <c r="D61" s="27" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E61" s="27"/>
       <c r="F61" s="28" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G61" s="78"/>
       <c r="H61" s="28"/>
@@ -5315,13 +5315,13 @@
       <c r="L61" s="28"/>
       <c r="M61" s="27"/>
       <c r="N61" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O61" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P61" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q61" s="28"/>
       <c r="R61" s="13"/>
@@ -5329,18 +5329,18 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="27" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="28" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G62" s="78"/>
       <c r="H62" s="28"/>
@@ -5350,13 +5350,13 @@
       <c r="L62" s="28"/>
       <c r="M62" s="27"/>
       <c r="N62" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O62" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P62" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q62" s="28"/>
       <c r="R62" s="13"/>
@@ -5364,20 +5364,20 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="38" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C63" s="39" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="E63" s="39"/>
       <c r="F63" s="40" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G63" s="80"/>
       <c r="H63" s="40"/>
@@ -5387,13 +5387,13 @@
       <c r="L63" s="40"/>
       <c r="M63" s="39"/>
       <c r="N63" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O63" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P63" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q63" s="40"/>
       <c r="R63" s="13"/>
@@ -5401,18 +5401,18 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C64" s="39"/>
       <c r="D64" s="39" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E64" s="39"/>
       <c r="F64" s="40" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="G64" s="80"/>
       <c r="H64" s="40"/>
@@ -5422,13 +5422,13 @@
       <c r="L64" s="40"/>
       <c r="M64" s="39"/>
       <c r="N64" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O64" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P64" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q64" s="40"/>
       <c r="R64" s="13"/>
@@ -5436,20 +5436,20 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E65" s="27"/>
       <c r="F65" s="28" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G65" s="78"/>
       <c r="H65" s="28"/>
@@ -5459,13 +5459,13 @@
       <c r="L65" s="28"/>
       <c r="M65" s="27"/>
       <c r="N65" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O65" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P65" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q65" s="28"/>
       <c r="R65" s="13"/>
@@ -5473,20 +5473,20 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E66" s="27"/>
       <c r="F66" s="28" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G66" s="78"/>
       <c r="H66" s="28"/>
@@ -5496,13 +5496,13 @@
       <c r="L66" s="28"/>
       <c r="M66" s="27"/>
       <c r="N66" s="29" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O66" s="28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P66" s="28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q66" s="28"/>
       <c r="R66" s="13"/>
@@ -5510,18 +5510,18 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="38" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C67" s="39"/>
       <c r="D67" s="39" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E67" s="39"/>
       <c r="F67" s="40" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="G67" s="80"/>
       <c r="H67" s="40"/>
@@ -5531,13 +5531,13 @@
       <c r="L67" s="40"/>
       <c r="M67" s="39"/>
       <c r="N67" s="41" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O67" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P67" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q67" s="40"/>
       <c r="R67" s="13"/>
@@ -5545,20 +5545,20 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="38" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B68" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="C68" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="C68" s="39" t="s">
-        <v>291</v>
-      </c>
       <c r="D68" s="39" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E68" s="39"/>
       <c r="F68" s="40" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G68" s="80"/>
       <c r="H68" s="40"/>
@@ -5568,13 +5568,13 @@
       <c r="L68" s="40"/>
       <c r="M68" s="39"/>
       <c r="N68" s="41" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O68" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P68" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q68" s="40"/>
       <c r="R68" s="13"/>
@@ -5582,20 +5582,20 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="38" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C69" s="39" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D69" s="39" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E69" s="39"/>
       <c r="F69" s="40" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G69" s="80"/>
       <c r="H69" s="40"/>
@@ -5605,13 +5605,13 @@
       <c r="L69" s="40"/>
       <c r="M69" s="39"/>
       <c r="N69" s="41" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O69" s="40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P69" s="40" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q69" s="40"/>
       <c r="R69" s="13"/>
@@ -5619,29 +5619,29 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E70" s="21"/>
       <c r="F70" s="22" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="G70" s="112">
         <v>3144</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="I70" s="102" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J70" s="24">
         <v>7</v>
@@ -5654,65 +5654,65 @@
         <v>5940</v>
       </c>
       <c r="N70" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O70" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P70" s="22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q70" s="22"/>
       <c r="R70" s="13"/>
       <c r="S70" s="118" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B71" s="44" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C71" s="44"/>
       <c r="D71" s="44" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="E71" s="44"/>
       <c r="F71" s="45" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="G71" s="81" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="I71" s="109" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J71" s="47">
         <v>63</v>
       </c>
       <c r="K71" s="44" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="L71" s="45"/>
       <c r="M71" s="44"/>
       <c r="N71" s="46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O71" s="45" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="P71" s="45" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q71" s="45"/>
       <c r="R71" s="13"/>
       <c r="S71" s="118" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -5720,52 +5720,52 @@
         <v>42</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="F72" s="22" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G72" s="75" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="H72" s="22" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="I72" s="102" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="J72" s="24">
         <v>4</v>
       </c>
       <c r="K72" s="21" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="L72" s="22"/>
       <c r="M72" s="21"/>
       <c r="N72" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O72" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P72" s="22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q72" s="22" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="R72" s="13"/>
       <c r="S72" s="118" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -5922,7 +5922,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="137" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B81" s="138"/>
       <c r="C81" s="138"/>
@@ -5945,29 +5945,29 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="55" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B82" s="63" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C82" s="63"/>
       <c r="D82" s="63" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="F82" s="64" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="G82" s="126">
         <v>8485</v>
       </c>
       <c r="H82" s="28" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="I82" s="107" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J82" s="73">
         <v>87</v>
@@ -5980,42 +5980,42 @@
         <v>40311</v>
       </c>
       <c r="N82" s="72" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="O82" s="64" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="P82" s="64" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="Q82" s="64" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="R82" s="65" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="S82" s="13" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="B83" s="61" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C83" s="61" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D83" s="61" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E83" s="61" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F83" s="62" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="G83" s="74"/>
       <c r="H83" s="8"/>
@@ -6025,35 +6025,35 @@
       <c r="L83" s="62"/>
       <c r="M83" s="61"/>
       <c r="N83" s="17" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="O83" s="62" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P83" s="62" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q83" s="62" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="R83" s="62" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="S83" s="13"/>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B84" s="49" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="C84" s="49"/>
       <c r="D84" s="49" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="E84" s="49" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="F84" s="13"/>
       <c r="G84" s="82"/>
@@ -6063,27 +6063,27 @@
       <c r="L84" s="13"/>
       <c r="M84" s="49"/>
       <c r="N84" s="50" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="O84" s="13" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="P84" s="13" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="Q84" s="13" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="R84" s="13" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="S84" s="13" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="85" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="128" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B85" s="129"/>
       <c r="C85" s="129"/>
@@ -6148,37 +6148,37 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="68" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B88" s="68" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C88" s="68" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="D88" s="68" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E88" s="68" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="F88" s="68" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G88" s="68" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="H88" s="68" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I88" s="68" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="J88" s="68" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K88" s="68" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="M88" s="68"/>
       <c r="N88" s="68"/>
@@ -6191,7 +6191,7 @@
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="68"/>
       <c r="B89" s="69" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C89" s="68">
         <v>3</v>
@@ -6200,7 +6200,7 @@
         <v>3</v>
       </c>
       <c r="E89" s="68" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="F89" s="68"/>
       <c r="G89" s="68"/>
@@ -6220,7 +6220,7 @@
     <row r="90" spans="1:20" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="69" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C90" s="69"/>
       <c r="D90" s="6"/>
@@ -6246,7 +6246,7 @@
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
       <c r="B91" s="69" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C91" s="20"/>
       <c r="D91" s="20"/>
@@ -6271,7 +6271,7 @@
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="71"/>
       <c r="B92" s="69" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C92" s="32">
         <v>2</v>
@@ -6282,7 +6282,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="32" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H92" s="32"/>
       <c r="I92" s="32"/>
@@ -6300,7 +6300,7 @@
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="38"/>
       <c r="B93" s="69" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C93" s="38">
         <v>14</v>
@@ -6325,7 +6325,7 @@
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="26"/>
       <c r="B94" s="69" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C94" s="26">
         <v>14</v>
@@ -6354,7 +6354,7 @@
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="92"/>
       <c r="B95" s="69" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C95" s="92"/>
       <c r="D95" s="92"/>

</xml_diff>

<commit_message>
finished comparedata function to be working with string non-numeric and numeric id's
</commit_message>
<xml_diff>
--- a/app/files/2021-StMM-Overzicht-Weezenkerkhof.xlsx
+++ b/app/files/2021-StMM-Overzicht-Weezenkerkhof.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\SSS-dev\webapplication-stichting-memento-mori\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A694B7-91FB-42AA-B277-CC8BBD963AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF4C7C-4D5E-47CA-A5CC-0B6B20F29420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CC40A5F-39CE-A24E-BAE0-2D8E0A6EA817}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="524">
   <si>
     <t>Periode</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Voorheen Weeskind</t>
   </si>
   <si>
-    <t xml:space="preserve">Schaik </t>
-  </si>
-  <si>
     <t>van</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>(1929-1994)</t>
   </si>
   <si>
-    <t>Dodewaard </t>
-  </si>
-  <si>
     <t>Eenpersoongraf</t>
   </si>
   <si>
@@ -289,9 +283,6 @@
     <t>(1902-1973)</t>
   </si>
   <si>
-    <t xml:space="preserve">11a  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Plas </t>
   </si>
   <si>
@@ -301,9 +292,6 @@
     <t>Hoofdonderwijzer</t>
   </si>
   <si>
-    <t xml:space="preserve">11b </t>
-  </si>
-  <si>
     <t xml:space="preserve">(van der Plas) - Rührwiem </t>
   </si>
   <si>
@@ -316,9 +304,6 @@
     <t>Leiden </t>
   </si>
   <si>
-    <t xml:space="preserve">11c  </t>
-  </si>
-  <si>
     <t>Plas</t>
   </si>
   <si>
@@ -334,9 +319,6 @@
     <t>Dochter</t>
   </si>
   <si>
-    <t xml:space="preserve">12  </t>
-  </si>
-  <si>
     <t>Veenstra</t>
   </si>
   <si>
@@ -352,9 +334,6 @@
     <t>Kind</t>
   </si>
   <si>
-    <t xml:space="preserve">13  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Wouw </t>
   </si>
   <si>
@@ -367,9 +346,6 @@
     <t>Capelle a/d IJssel </t>
   </si>
   <si>
-    <t xml:space="preserve">14  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Knippers </t>
   </si>
   <si>
@@ -382,9 +358,6 @@
     <t>Zeist </t>
   </si>
   <si>
-    <t>15 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lindenhout </t>
   </si>
   <si>
@@ -397,9 +370,6 @@
     <t>(1836-1918)</t>
   </si>
   <si>
-    <t xml:space="preserve">16  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hendrina </t>
   </si>
   <si>
@@ -418,18 +388,12 @@
     <t>(1828-1907)</t>
   </si>
   <si>
-    <t xml:space="preserve">18a  </t>
-  </si>
-  <si>
     <t>Sophia Maria Mathilda</t>
   </si>
   <si>
     <t>(1855-1907)</t>
   </si>
   <si>
-    <t xml:space="preserve">18b  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Belonje </t>
   </si>
   <si>
@@ -463,9 +427,6 @@
     <t>(1854-1902)</t>
   </si>
   <si>
-    <t xml:space="preserve">20  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Belmer </t>
   </si>
   <si>
@@ -484,9 +445,6 @@
     <t>(1852-1896)</t>
   </si>
   <si>
-    <t>22 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Geerdes </t>
   </si>
   <si>
@@ -508,9 +466,6 @@
     <t xml:space="preserve">(1868-1921)  </t>
   </si>
   <si>
-    <t xml:space="preserve">23b </t>
-  </si>
-  <si>
     <t>de</t>
   </si>
   <si>
@@ -526,9 +481,6 @@
     <t>(1862-1922)</t>
   </si>
   <si>
-    <t xml:space="preserve">25  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Becker </t>
   </si>
   <si>
@@ -553,9 +505,6 @@
     <t>(1874 -1964)</t>
   </si>
   <si>
-    <t xml:space="preserve">27   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Kooper </t>
   </si>
   <si>
@@ -565,9 +514,6 @@
     <t>(1897 -1945)</t>
   </si>
   <si>
-    <t xml:space="preserve">28  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bokelaar </t>
   </si>
   <si>
@@ -586,9 +532,6 @@
     <t>(1937-1947)</t>
   </si>
   <si>
-    <t>30a </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vermeulen </t>
   </si>
   <si>
@@ -598,9 +541,6 @@
     <t>(1926-1940)</t>
   </si>
   <si>
-    <t>30b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Jonkergouw </t>
   </si>
   <si>
@@ -619,18 +559,12 @@
     <t>(1926-1944)</t>
   </si>
   <si>
-    <t xml:space="preserve">31a  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hendrika </t>
   </si>
   <si>
     <t>(1915-1936)</t>
   </si>
   <si>
-    <t xml:space="preserve">31b  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Kok </t>
   </si>
   <si>
@@ -643,45 +577,30 @@
     <t>Kind/ Helpster</t>
   </si>
   <si>
-    <t xml:space="preserve">31c  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Schimmel </t>
   </si>
   <si>
     <t>(1916-1938)</t>
   </si>
   <si>
-    <t xml:space="preserve">32a  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Arnold </t>
   </si>
   <si>
     <t>(1930-1935)</t>
   </si>
   <si>
-    <t>32b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Boekee </t>
   </si>
   <si>
     <t>(1919-1935)</t>
   </si>
   <si>
-    <t xml:space="preserve">32c  </t>
-  </si>
-  <si>
     <t>Scholtens</t>
   </si>
   <si>
     <t>(1932-1936)</t>
   </si>
   <si>
-    <t xml:space="preserve">33a  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rutten </t>
   </si>
   <si>
@@ -706,27 +625,18 @@
     <t>(1916 -1935)</t>
   </si>
   <si>
-    <t xml:space="preserve">34  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mons </t>
   </si>
   <si>
     <t>(1930-1931)</t>
   </si>
   <si>
-    <t xml:space="preserve">35a </t>
-  </si>
-  <si>
     <t xml:space="preserve">Beck </t>
   </si>
   <si>
     <t xml:space="preserve">Nicolaas J. </t>
   </si>
   <si>
-    <t xml:space="preserve">35b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Majoor </t>
   </si>
   <si>
@@ -742,9 +652,6 @@
     <t>(1913 -1929)</t>
   </si>
   <si>
-    <t xml:space="preserve">36b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Waasdorp </t>
   </si>
   <si>
@@ -754,9 +661,6 @@
     <t>(1926-1930)</t>
   </si>
   <si>
-    <t xml:space="preserve">36c </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vrijenhoek </t>
   </si>
   <si>
@@ -766,9 +670,6 @@
     <t>(1917-1931)</t>
   </si>
   <si>
-    <t>37a </t>
-  </si>
-  <si>
     <t xml:space="preserve">Harskamp </t>
   </si>
   <si>
@@ -778,9 +679,6 @@
     <t>(1912-1931)</t>
   </si>
   <si>
-    <t>37b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Muyzert </t>
   </si>
   <si>
@@ -790,9 +688,6 @@
     <t>(1912 -1932)</t>
   </si>
   <si>
-    <t>37c </t>
-  </si>
-  <si>
     <t xml:space="preserve">Beek </t>
   </si>
   <si>
@@ -805,9 +700,6 @@
     <t>(1916-1932)</t>
   </si>
   <si>
-    <t>38a </t>
-  </si>
-  <si>
     <t xml:space="preserve">Brussee </t>
   </si>
   <si>
@@ -817,9 +709,6 @@
     <t>(1911-1932)</t>
   </si>
   <si>
-    <t>38b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Johannes </t>
   </si>
   <si>
@@ -838,9 +727,6 @@
     <t>(1922-1933)</t>
   </si>
   <si>
-    <t>39a </t>
-  </si>
-  <si>
     <t xml:space="preserve">Spaans </t>
   </si>
   <si>
@@ -850,9 +736,6 @@
     <t>(1915 -1933)</t>
   </si>
   <si>
-    <t>39b </t>
-  </si>
-  <si>
     <t xml:space="preserve">van der </t>
   </si>
   <si>
@@ -862,18 +745,12 @@
     <t>(1914-1933)</t>
   </si>
   <si>
-    <t xml:space="preserve">39c  </t>
-  </si>
-  <si>
     <t>van de</t>
   </si>
   <si>
     <t>(1920-1934)</t>
   </si>
   <si>
-    <t xml:space="preserve">40  </t>
-  </si>
-  <si>
     <t>Beek</t>
   </si>
   <si>
@@ -883,9 +760,6 @@
     <t>(1908 -1916)</t>
   </si>
   <si>
-    <t>41 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Molijn </t>
   </si>
   <si>
@@ -1126,9 +1000,6 @@
     <t>26b</t>
   </si>
   <si>
-    <t xml:space="preserve">26c  </t>
-  </si>
-  <si>
     <t>Voogdykind</t>
   </si>
   <si>
@@ -1643,6 +1514,96 @@
   </si>
   <si>
     <t>20/03/1869</t>
+  </si>
+  <si>
+    <t>Schaik</t>
+  </si>
+  <si>
+    <t>Dodewaard</t>
+  </si>
+  <si>
+    <t>31c</t>
+  </si>
+  <si>
+    <t>11a</t>
+  </si>
+  <si>
+    <t>11b</t>
+  </si>
+  <si>
+    <t>11c</t>
+  </si>
+  <si>
+    <t>18a</t>
+  </si>
+  <si>
+    <t>18b</t>
+  </si>
+  <si>
+    <t>23b</t>
+  </si>
+  <si>
+    <t>26c</t>
+  </si>
+  <si>
+    <t>30a</t>
+  </si>
+  <si>
+    <t>30b</t>
+  </si>
+  <si>
+    <t>31a</t>
+  </si>
+  <si>
+    <t>31b</t>
+  </si>
+  <si>
+    <t>32a</t>
+  </si>
+  <si>
+    <t>32b</t>
+  </si>
+  <si>
+    <t>32c</t>
+  </si>
+  <si>
+    <t>33a</t>
+  </si>
+  <si>
+    <t>35a</t>
+  </si>
+  <si>
+    <t>35b</t>
+  </si>
+  <si>
+    <t>36b</t>
+  </si>
+  <si>
+    <t>36c</t>
+  </si>
+  <si>
+    <t>37a</t>
+  </si>
+  <si>
+    <t>37b</t>
+  </si>
+  <si>
+    <t>37c</t>
+  </si>
+  <si>
+    <t>38a</t>
+  </si>
+  <si>
+    <t>38b</t>
+  </si>
+  <si>
+    <t>39a</t>
+  </si>
+  <si>
+    <t>39b</t>
+  </si>
+  <si>
+    <t>39c</t>
   </si>
 </sst>
 </file>
@@ -2387,8 +2348,8 @@
   <dimension ref="A1:T414"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2418,49 +2379,49 @@
   <sheetData>
     <row r="1" spans="1:20" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>406</v>
+        <v>363</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>407</v>
+        <v>364</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>408</v>
+        <v>365</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>409</v>
+        <v>366</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>404</v>
+        <v>361</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>410</v>
+        <v>367</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>412</v>
+        <v>369</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>405</v>
+        <v>362</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>413</v>
+        <v>370</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>414</v>
+        <v>371</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2</v>
@@ -2469,10 +2430,10 @@
         <v>3</v>
       </c>
       <c r="R1" s="75" t="s">
-        <v>415</v>
+        <v>372</v>
       </c>
       <c r="S1" s="76" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="T1" s="78"/>
     </row>
@@ -2481,313 +2442,313 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="80" t="s">
-        <v>416</v>
+        <v>373</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>9</v>
+        <v>495</v>
       </c>
       <c r="I2" s="64" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J2" s="10">
         <v>65</v>
       </c>
       <c r="K2" s="81" t="s">
-        <v>417</v>
+        <v>374</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>411</v>
+        <v>368</v>
       </c>
       <c r="M2" s="83" t="s">
-        <v>417</v>
+        <v>374</v>
       </c>
       <c r="N2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="R2" s="85" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="S2" s="77"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3" s="64" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J3" s="13">
         <v>79</v>
       </c>
       <c r="K3" s="81" t="s">
-        <v>420</v>
+        <v>377</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="82" t="s">
-        <v>421</v>
+        <v>378</v>
       </c>
       <c r="N3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="77"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="86" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="J4" s="14">
         <v>90</v>
       </c>
       <c r="K4" s="83" t="s">
-        <v>528</v>
+        <v>485</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="83" t="s">
-        <v>533</v>
+        <v>490</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>329</v>
+        <v>287</v>
       </c>
       <c r="R4" s="11"/>
       <c r="S4" s="77"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="80" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I5" s="64" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J5" s="10">
         <v>68</v>
       </c>
       <c r="K5" s="83" t="s">
-        <v>527</v>
+        <v>484</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="83" t="s">
-        <v>534</v>
+        <v>491</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R5" s="11"/>
       <c r="S5" s="77"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" s="87" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="J6" s="15">
         <v>99</v>
       </c>
       <c r="K6" s="83" t="s">
-        <v>532</v>
+        <v>489</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="M6" s="83" t="s">
-        <v>535</v>
+        <v>492</v>
       </c>
       <c r="N6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R6" s="11"/>
       <c r="S6" s="77" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G7" s="88" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="I7" s="66" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J7" s="20">
         <v>58</v>
       </c>
       <c r="K7" s="103" t="s">
-        <v>531</v>
+        <v>488</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="M7" s="103" t="s">
-        <v>535</v>
+        <v>492</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R7" s="11"/>
       <c r="S7" s="77" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2795,48 +2756,48 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="89" t="s">
+        <v>383</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="89" t="s">
-        <v>426</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="I8" s="64" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="J8" s="15">
         <v>78</v>
       </c>
       <c r="K8" s="83" t="s">
-        <v>530</v>
+        <v>487</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>299</v>
+        <v>257</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R8" s="11"/>
       <c r="S8" s="77"/>
@@ -2846,48 +2807,48 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="G9" s="90" t="s">
+        <v>384</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="90" t="s">
-        <v>427</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="I9" s="64" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J9" s="15">
         <v>64</v>
       </c>
       <c r="K9" s="83" t="s">
-        <v>529</v>
+        <v>486</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="7"/>
       <c r="N9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q9" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R9" s="11"/>
       <c r="S9" s="77"/>
@@ -2897,770 +2858,770 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>385</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="90" t="s">
-        <v>428</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="I10" s="64" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="J10" s="15">
         <v>43</v>
       </c>
       <c r="K10" s="83" t="s">
-        <v>460</v>
+        <v>417</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="M10" s="83" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="N10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q10" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R10" s="11"/>
       <c r="S10" s="77"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G11" s="90" t="s">
-        <v>429</v>
+        <v>386</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I11" s="64" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="J11" s="15">
         <v>69</v>
       </c>
       <c r="K11" s="83" t="s">
-        <v>461</v>
+        <v>418</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>301</v>
+        <v>259</v>
       </c>
       <c r="M11" s="83" t="s">
-        <v>494</v>
+        <v>451</v>
       </c>
       <c r="N11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R11" s="74"/>
       <c r="S11" s="77"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="G12" s="90" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J12" s="15">
         <v>76</v>
       </c>
       <c r="K12" s="83" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>303</v>
+        <v>261</v>
       </c>
       <c r="M12" s="83" t="s">
-        <v>495</v>
+        <v>452</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="R12" s="74"/>
       <c r="S12" s="77"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="96" t="s">
-        <v>463</v>
+        <v>420</v>
       </c>
       <c r="G13" s="90" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J13" s="15">
         <v>74</v>
       </c>
       <c r="K13" s="83" t="s">
-        <v>464</v>
+        <v>421</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="83" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="N13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q13" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R13" s="74"/>
       <c r="S13" s="77"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="90" t="s">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="I14" s="64" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="J14" s="15">
         <v>62</v>
       </c>
       <c r="K14" s="83" t="s">
-        <v>465</v>
+        <v>422</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="83" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R14" s="11"/>
       <c r="S14" s="77"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" s="90" t="s">
-        <v>433</v>
+        <v>390</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I15" s="64" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="J15" s="15">
         <v>63</v>
       </c>
       <c r="K15" s="83" t="s">
-        <v>466</v>
+        <v>423</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="83" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="N15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q15" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R15" s="11"/>
       <c r="S15" s="77"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G16" s="90" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I16" s="64" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="J16" s="15">
         <v>71</v>
       </c>
       <c r="K16" s="83" t="s">
-        <v>467</v>
+        <v>424</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="83" t="s">
-        <v>499</v>
+        <v>456</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="R16" s="11"/>
       <c r="S16" s="77"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>85</v>
+        <v>497</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G17" s="90" t="s">
-        <v>435</v>
+        <v>392</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I17" s="64" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J17" s="15">
         <v>55</v>
       </c>
       <c r="K17" s="83" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="83" t="s">
-        <v>500</v>
+        <v>457</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R17" s="11"/>
       <c r="S17" s="77"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>498</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G18" s="90" t="s">
-        <v>436</v>
+        <v>393</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I18" s="64" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J18" s="15">
         <v>67</v>
       </c>
       <c r="K18" s="83" t="s">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="83" t="s">
-        <v>501</v>
+        <v>458</v>
       </c>
       <c r="N18" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="77"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>94</v>
+        <v>499</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G19" s="88" t="s">
-        <v>437</v>
+        <v>394</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I19" s="66" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J19" s="20">
         <v>53</v>
       </c>
       <c r="K19" s="97" t="s">
-        <v>470</v>
+        <v>427</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="17"/>
       <c r="N19" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P19" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R19" s="11"/>
       <c r="S19" s="77"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>100</v>
+      <c r="A20" s="22">
+        <v>12</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G20" s="91" t="s">
-        <v>438</v>
+        <v>395</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I20" s="67" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
       <c r="J20" s="27">
         <v>14</v>
       </c>
       <c r="K20" s="98" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
       <c r="M20" s="98" t="s">
-        <v>502</v>
+        <v>459</v>
       </c>
       <c r="N20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="P20" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O20" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="P20" s="24" t="s">
-        <v>12</v>
-      </c>
       <c r="Q20" s="24" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="R20" s="11"/>
       <c r="S20" s="77" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>106</v>
+      <c r="A21" s="6">
+        <v>13</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G21" s="90" t="s">
-        <v>439</v>
+        <v>396</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="J21" s="15">
         <v>54</v>
       </c>
       <c r="K21" s="83" t="s">
-        <v>472</v>
+        <v>429</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="83" t="s">
-        <v>503</v>
+        <v>460</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="R21" s="108" t="s">
-        <v>526</v>
+        <v>483</v>
       </c>
       <c r="S21" s="77"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>111</v>
+      <c r="A22" s="6">
+        <v>14</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G22" s="90" t="s">
-        <v>440</v>
+        <v>397</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I22" s="64" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="J22" s="15">
         <v>37</v>
       </c>
       <c r="K22" s="83" t="s">
-        <v>473</v>
+        <v>430</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>304</v>
+        <v>262</v>
       </c>
       <c r="M22" s="83" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="N22" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q22" s="8" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
       <c r="R22" s="11"/>
       <c r="S22" s="77"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>116</v>
+      <c r="A23" s="49">
+        <v>15</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E23" s="54"/>
       <c r="F23" s="47" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G23" s="93" t="s">
-        <v>441</v>
+        <v>398</v>
       </c>
       <c r="H23" s="55" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I23" s="68" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J23" s="56">
         <v>81</v>
       </c>
       <c r="K23" s="99" t="s">
-        <v>474</v>
+        <v>431</v>
       </c>
       <c r="L23" s="47" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="M23" s="99" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="N23" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="P23" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="O23" s="47" t="s">
-        <v>333</v>
-      </c>
-      <c r="P23" s="47" t="s">
-        <v>12</v>
-      </c>
       <c r="Q23" s="47" t="s">
-        <v>399</v>
+        <v>356</v>
       </c>
       <c r="R23" s="11"/>
       <c r="S23" s="77" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
-        <v>121</v>
+      <c r="A24" s="49">
+        <v>16</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="C24" s="54"/>
       <c r="D24" s="54" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E24" s="54"/>
       <c r="F24" s="47" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G24" s="94" t="s">
-        <v>442</v>
+        <v>399</v>
       </c>
       <c r="H24" s="55" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="I24" s="68" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J24" s="56">
         <v>63</v>
       </c>
       <c r="K24" s="99" t="s">
-        <v>475</v>
+        <v>432</v>
       </c>
       <c r="L24" s="47"/>
       <c r="M24" s="54"/>
       <c r="N24" s="57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O24" s="47" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="P24" s="47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q24" s="47" t="s">
-        <v>400</v>
+        <v>357</v>
       </c>
       <c r="R24" s="11"/>
       <c r="S24" s="77" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -3668,299 +3629,299 @@
         <v>17</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G25" s="89" t="s">
-        <v>443</v>
+        <v>400</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I25" s="65" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J25" s="15">
         <v>79</v>
       </c>
       <c r="K25" s="83" t="s">
-        <v>476</v>
+        <v>433</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="83" t="s">
-        <v>506</v>
+        <v>463</v>
       </c>
       <c r="N25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q25" s="8" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="R25" s="11"/>
       <c r="S25" s="77"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>128</v>
+        <v>500</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="8" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G26" s="89" t="s">
-        <v>444</v>
+        <v>401</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="I26" s="65" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J26" s="15">
         <v>51</v>
       </c>
       <c r="K26" s="83" t="s">
-        <v>477</v>
+        <v>434</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>308</v>
+        <v>266</v>
       </c>
       <c r="M26" s="83" t="s">
-        <v>507</v>
+        <v>464</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q26" s="8" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="R26" s="11"/>
       <c r="S26" s="77"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>131</v>
+        <v>501</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="G27" s="89" t="s">
-        <v>445</v>
+        <v>402</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>309</v>
+        <v>267</v>
       </c>
       <c r="I27" s="65" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="J27" s="15">
         <v>74</v>
       </c>
       <c r="K27" s="83" t="s">
-        <v>478</v>
+        <v>435</v>
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="83" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
       <c r="N27" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="R27" s="11"/>
       <c r="S27" s="77"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="30" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="G28" s="92" t="s">
-        <v>446</v>
+        <v>403</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J28" s="32">
         <v>55</v>
       </c>
       <c r="K28" s="100" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="L28" s="30" t="s">
-        <v>337</v>
+        <v>295</v>
       </c>
       <c r="M28" s="29"/>
       <c r="N28" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O28" s="30" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="P28" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q28" s="30" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="R28" s="11"/>
       <c r="S28" s="77"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="30" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G29" s="92" t="s">
-        <v>447</v>
+        <v>404</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="I29" s="69" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J29" s="32">
         <v>68</v>
       </c>
       <c r="K29" s="101" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="L29" s="30" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
       <c r="M29" s="29"/>
       <c r="N29" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O29" s="30" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="P29" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q29" s="30" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="R29" s="11"/>
       <c r="S29" s="77"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>143</v>
+      <c r="A30" s="6">
+        <v>20</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="8" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="G30" s="89" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="I30" s="65" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J30" s="15">
         <v>90</v>
       </c>
       <c r="K30" s="82" t="s">
-        <v>480</v>
+        <v>437</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>310</v>
+        <v>268</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O30" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q30" s="8" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="R30" s="11"/>
       <c r="S30" s="77" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -3968,197 +3929,197 @@
         <v>21</v>
       </c>
       <c r="B31" s="60" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C31" s="60"/>
       <c r="D31" s="60" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E31" s="60"/>
       <c r="F31" s="61" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="G31" s="95" t="s">
-        <v>449</v>
+        <v>406</v>
       </c>
       <c r="H31" s="61" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="I31" s="70" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="J31" s="62">
         <v>44</v>
       </c>
       <c r="K31" s="102" t="s">
-        <v>481</v>
+        <v>438</v>
       </c>
       <c r="L31" s="61" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="M31" s="60"/>
       <c r="N31" s="63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O31" s="61" t="s">
         <v>4</v>
       </c>
       <c r="P31" s="61" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q31" s="61" t="s">
-        <v>401</v>
+        <v>358</v>
       </c>
       <c r="R31" s="59"/>
       <c r="S31" s="77"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>150</v>
+      <c r="A32" s="6">
+        <v>22</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="8" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="G32" s="89" t="s">
-        <v>450</v>
+        <v>407</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
       <c r="I32" s="65" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J32" s="15">
         <v>52</v>
       </c>
       <c r="K32" s="82" t="s">
-        <v>482</v>
+        <v>439</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>312</v>
+        <v>270</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P32" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q32" s="8" t="s">
-        <v>397</v>
+        <v>354</v>
       </c>
       <c r="R32" s="11"/>
       <c r="S32" s="77"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="8" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G33" s="89" t="s">
-        <v>451</v>
+        <v>408</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I33" s="65" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="J33" s="15">
         <v>51</v>
       </c>
       <c r="K33" s="83" t="s">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>313</v>
+        <v>271</v>
       </c>
       <c r="M33" s="83" t="s">
-        <v>509</v>
+        <v>466</v>
       </c>
       <c r="N33" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P33" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q33" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R33" s="11"/>
       <c r="S33" s="77"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>158</v>
+        <v>502</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>296</v>
+        <v>254</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="8" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="G34" s="89" t="s">
-        <v>536</v>
+        <v>493</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>314</v>
+        <v>272</v>
       </c>
       <c r="I34" s="65" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J34" s="15">
         <v>80</v>
       </c>
       <c r="K34" s="83" t="s">
-        <v>484</v>
+        <v>441</v>
       </c>
       <c r="L34" s="8"/>
       <c r="M34" s="83" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="N34" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q34" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q34" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="R34" s="11"/>
       <c r="S34" s="77"/>
@@ -4168,348 +4129,348 @@
         <v>24</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>384</v>
+        <v>341</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="8" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="G35" s="89" t="s">
-        <v>452</v>
+        <v>409</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J35" s="15">
         <v>59</v>
       </c>
       <c r="K35" s="83" t="s">
-        <v>485</v>
+        <v>442</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
       <c r="M35" s="83" t="s">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="N35" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="R35" s="11"/>
       <c r="S35" s="77"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>164</v>
+      <c r="A36" s="6">
+        <v>25</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="8" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G36" s="89" t="s">
-        <v>455</v>
+        <v>412</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="I36" s="65" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="J36" s="15">
         <v>50</v>
       </c>
       <c r="K36" s="83" t="s">
-        <v>486</v>
+        <v>443</v>
       </c>
       <c r="L36" s="8"/>
       <c r="M36" s="83" t="s">
-        <v>512</v>
+        <v>469</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q36" s="8" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="R36" s="11"/>
       <c r="S36" s="77"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>297</v>
+        <v>255</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="8" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="G37" s="89" t="s">
-        <v>456</v>
+        <v>413</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I37" s="65" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J37" s="15">
         <v>63</v>
       </c>
       <c r="K37" s="83" t="s">
-        <v>487</v>
+        <v>444</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="M37" s="83" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O37" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q37" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R37" s="11"/>
       <c r="S37" s="77"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="18" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="G38" s="88" t="s">
-        <v>453</v>
+        <v>410</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="I38" s="66" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J38" s="20">
         <v>41</v>
       </c>
       <c r="K38" s="103" t="s">
-        <v>488</v>
+        <v>445</v>
       </c>
       <c r="L38" s="18"/>
       <c r="M38" s="103" t="s">
-        <v>514</v>
+        <v>471</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P38" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q38" s="18" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
       <c r="R38" s="11"/>
       <c r="S38" s="77"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>364</v>
+        <v>503</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="8" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="G39" s="89" t="s">
-        <v>457</v>
+        <v>414</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="I39" s="65" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J39" s="15">
         <v>89</v>
       </c>
       <c r="K39" s="83" t="s">
-        <v>489</v>
+        <v>446</v>
       </c>
       <c r="L39" s="8"/>
       <c r="M39" s="83" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q39" s="8" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
       <c r="R39" s="11"/>
       <c r="S39" s="77"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>173</v>
+      <c r="A40" s="6">
+        <v>27</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="8" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="G40" s="89" t="s">
-        <v>458</v>
+        <v>415</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="I40" s="65" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="J40" s="15">
         <v>47</v>
       </c>
       <c r="K40" s="83" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="M40" s="83" t="s">
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="N40" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P40" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P40" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q40" s="8" t="s">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="R40" s="11"/>
       <c r="S40" s="77"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>177</v>
+      <c r="A41" s="6">
+        <v>28</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="8" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="G41" s="89" t="s">
-        <v>459</v>
+        <v>416</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
       <c r="I41" s="65" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="J41" s="15">
         <v>58</v>
       </c>
       <c r="K41" s="83" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>327</v>
+        <v>285</v>
       </c>
       <c r="M41" s="83" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="N41" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O41" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P41" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="Q41" s="8" t="s">
-        <v>328</v>
+        <v>286</v>
       </c>
       <c r="R41" s="11"/>
       <c r="S41" s="77"/>
@@ -4519,72 +4480,72 @@
         <v>29</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E42" s="23"/>
       <c r="F42" s="24" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="G42" s="91" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="I42" s="71" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J42" s="27">
         <v>10</v>
       </c>
       <c r="K42" s="98" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="M42" s="98" t="s">
-        <v>518</v>
+        <v>475</v>
       </c>
       <c r="N42" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O42" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="P42" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O42" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="P42" s="24" t="s">
-        <v>12</v>
-      </c>
       <c r="Q42" s="24" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="R42" s="11"/>
       <c r="S42" s="77" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>184</v>
+        <v>504</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="G43" s="52"/>
       <c r="H43" s="24"/>
@@ -4594,13 +4555,13 @@
       <c r="L43" s="24"/>
       <c r="M43" s="23"/>
       <c r="N43" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O43" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P43" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q43" s="24"/>
       <c r="R43" s="11"/>
@@ -4608,20 +4569,20 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>188</v>
+        <v>505</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="23" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="G44" s="52"/>
       <c r="H44" s="24"/>
@@ -4633,13 +4594,13 @@
       <c r="L44" s="24"/>
       <c r="M44" s="23"/>
       <c r="N44" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P44" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q44" s="24"/>
       <c r="R44" s="11"/>
@@ -4647,20 +4608,20 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="23" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="G45" s="52"/>
       <c r="H45" s="24"/>
@@ -4670,42 +4631,42 @@
       </c>
       <c r="K45" s="23"/>
       <c r="L45" s="24" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="M45" s="23"/>
       <c r="N45" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P45" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q45" s="24" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="R45" s="11"/>
       <c r="S45" s="77"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>195</v>
+        <v>506</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>395</v>
+        <v>352</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G46" s="53"/>
       <c r="H46" s="35"/>
@@ -4715,13 +4676,13 @@
       <c r="L46" s="35"/>
       <c r="M46" s="34"/>
       <c r="N46" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O46" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P46" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q46" s="35"/>
       <c r="R46" s="11"/>
@@ -4729,20 +4690,20 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>198</v>
+        <v>507</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="C47" s="34"/>
       <c r="D47" s="34" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="G47" s="53"/>
       <c r="H47" s="35"/>
@@ -4752,13 +4713,13 @@
       <c r="L47" s="35"/>
       <c r="M47" s="34"/>
       <c r="N47" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O47" s="35" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="P47" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q47" s="35"/>
       <c r="R47" s="11"/>
@@ -4766,18 +4727,18 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>203</v>
+        <v>496</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="23" t="s">
-        <v>331</v>
+        <v>289</v>
       </c>
       <c r="E48" s="23"/>
       <c r="F48" s="24" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="G48" s="52"/>
       <c r="H48" s="24"/>
@@ -4787,13 +4748,13 @@
       <c r="L48" s="24"/>
       <c r="M48" s="23"/>
       <c r="N48" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O48" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P48" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q48" s="24"/>
       <c r="R48" s="11"/>
@@ -4801,20 +4762,20 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>206</v>
+        <v>508</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="23" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>391</v>
+        <v>348</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="G49" s="52"/>
       <c r="H49" s="24"/>
@@ -4824,13 +4785,13 @@
       <c r="L49" s="24"/>
       <c r="M49" s="23"/>
       <c r="N49" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P49" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q49" s="24"/>
       <c r="R49" s="11"/>
@@ -4838,20 +4799,20 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
-        <v>209</v>
+        <v>509</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="C50" s="34"/>
       <c r="D50" s="34" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="F50" s="35" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="G50" s="53"/>
       <c r="H50" s="35"/>
@@ -4861,13 +4822,13 @@
       <c r="L50" s="35"/>
       <c r="M50" s="34"/>
       <c r="N50" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O50" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P50" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q50" s="35"/>
       <c r="R50" s="11"/>
@@ -4875,18 +4836,18 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>212</v>
+        <v>510</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="C51" s="34"/>
       <c r="D51" s="34" t="s">
-        <v>382</v>
+        <v>339</v>
       </c>
       <c r="E51" s="34"/>
       <c r="F51" s="35" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="G51" s="53"/>
       <c r="H51" s="35"/>
@@ -4896,13 +4857,13 @@
       <c r="L51" s="35"/>
       <c r="M51" s="34"/>
       <c r="N51" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O51" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P51" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q51" s="35"/>
       <c r="R51" s="11"/>
@@ -4910,20 +4871,20 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>215</v>
+        <v>511</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="23" t="s">
-        <v>383</v>
+        <v>340</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>392</v>
+        <v>349</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="G52" s="52"/>
       <c r="H52" s="24"/>
@@ -4933,13 +4894,13 @@
       <c r="L52" s="24"/>
       <c r="M52" s="23"/>
       <c r="N52" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O52" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P52" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q52" s="24"/>
       <c r="R52" s="11"/>
@@ -4947,18 +4908,18 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="C53" s="34"/>
       <c r="D53" s="34" t="s">
-        <v>381</v>
+        <v>338</v>
       </c>
       <c r="E53" s="34"/>
       <c r="F53" s="35" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="G53" s="53"/>
       <c r="H53" s="35"/>
@@ -4968,13 +4929,13 @@
       <c r="L53" s="35"/>
       <c r="M53" s="34"/>
       <c r="N53" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O53" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P53" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q53" s="35"/>
       <c r="R53" s="11"/>
@@ -4982,20 +4943,20 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="C54" s="34"/>
       <c r="D54" s="34" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="F54" s="35" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="G54" s="53"/>
       <c r="H54" s="35"/>
@@ -5005,34 +4966,34 @@
       <c r="L54" s="35"/>
       <c r="M54" s="34"/>
       <c r="N54" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O54" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P54" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q54" s="35"/>
       <c r="R54" s="11"/>
       <c r="S54" s="77"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>224</v>
+      <c r="A55" s="16">
+        <v>34</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17" t="s">
-        <v>379</v>
+        <v>336</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="G55" s="51"/>
       <c r="H55" s="18"/>
@@ -5042,34 +5003,34 @@
       <c r="L55" s="18"/>
       <c r="M55" s="17"/>
       <c r="N55" s="25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O55" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P55" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q55" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R55" s="11"/>
       <c r="S55" s="77"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>227</v>
+        <v>512</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="C56" s="23"/>
       <c r="D56" s="23" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="E56" s="23"/>
       <c r="F56" s="24" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="G56" s="52"/>
       <c r="H56" s="24"/>
@@ -5079,13 +5040,13 @@
       <c r="L56" s="24"/>
       <c r="M56" s="23"/>
       <c r="N56" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O56" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P56" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q56" s="24"/>
       <c r="R56" s="11"/>
@@ -5093,18 +5054,18 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
-        <v>230</v>
+        <v>513</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="C57" s="34"/>
       <c r="D57" s="34" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="E57" s="34"/>
       <c r="F57" s="35" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="G57" s="53"/>
       <c r="H57" s="35"/>
@@ -5114,13 +5075,13 @@
       <c r="L57" s="35"/>
       <c r="M57" s="34"/>
       <c r="N57" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O57" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P57" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q57" s="35"/>
       <c r="R57" s="11"/>
@@ -5128,20 +5089,20 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
-        <v>402</v>
+        <v>359</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E58" s="23"/>
       <c r="F58" s="24" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="G58" s="52"/>
       <c r="H58" s="24"/>
@@ -5151,13 +5112,13 @@
       <c r="L58" s="24"/>
       <c r="M58" s="23"/>
       <c r="N58" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O58" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P58" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q58" s="24"/>
       <c r="R58" s="11"/>
@@ -5165,18 +5126,18 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
-        <v>236</v>
+        <v>514</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="C59" s="34"/>
       <c r="D59" s="34" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="E59" s="34"/>
       <c r="F59" s="35" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="G59" s="53"/>
       <c r="H59" s="35"/>
@@ -5186,13 +5147,13 @@
       <c r="L59" s="35"/>
       <c r="M59" s="34"/>
       <c r="N59" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O59" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P59" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q59" s="35"/>
       <c r="R59" s="11"/>
@@ -5200,18 +5161,18 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
-        <v>240</v>
+        <v>515</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="C60" s="34"/>
       <c r="D60" s="34" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="E60" s="34"/>
       <c r="F60" s="35" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="G60" s="53"/>
       <c r="H60" s="35"/>
@@ -5221,13 +5182,13 @@
       <c r="L60" s="35"/>
       <c r="M60" s="34"/>
       <c r="N60" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O60" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P60" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q60" s="35"/>
       <c r="R60" s="11"/>
@@ -5235,18 +5196,18 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>244</v>
+        <v>516</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="C61" s="23"/>
       <c r="D61" s="23" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
       <c r="E61" s="23"/>
       <c r="F61" s="24" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="G61" s="52"/>
       <c r="H61" s="24"/>
@@ -5256,13 +5217,13 @@
       <c r="L61" s="24"/>
       <c r="M61" s="23"/>
       <c r="N61" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O61" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P61" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="11"/>
@@ -5270,18 +5231,18 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
-        <v>248</v>
+        <v>517</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="23" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="E62" s="23"/>
       <c r="F62" s="24" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="G62" s="52"/>
       <c r="H62" s="24"/>
@@ -5291,13 +5252,13 @@
       <c r="L62" s="24"/>
       <c r="M62" s="23"/>
       <c r="N62" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O62" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P62" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q62" s="24"/>
       <c r="R62" s="11"/>
@@ -5305,20 +5266,20 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
-        <v>252</v>
+        <v>518</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="E63" s="34"/>
       <c r="F63" s="35" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="G63" s="53"/>
       <c r="H63" s="35"/>
@@ -5328,13 +5289,13 @@
       <c r="L63" s="35"/>
       <c r="M63" s="34"/>
       <c r="N63" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O63" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P63" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q63" s="35"/>
       <c r="R63" s="11"/>
@@ -5342,18 +5303,18 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="33" t="s">
-        <v>257</v>
+        <v>519</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="C64" s="34"/>
       <c r="D64" s="34" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="E64" s="34"/>
       <c r="F64" s="35" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="G64" s="53"/>
       <c r="H64" s="35"/>
@@ -5363,13 +5324,13 @@
       <c r="L64" s="35"/>
       <c r="M64" s="34"/>
       <c r="N64" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O64" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P64" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q64" s="35"/>
       <c r="R64" s="11"/>
@@ -5377,20 +5338,20 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
-        <v>261</v>
+        <v>520</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="E65" s="23"/>
       <c r="F65" s="24" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="G65" s="52"/>
       <c r="H65" s="24"/>
@@ -5400,13 +5361,13 @@
       <c r="L65" s="24"/>
       <c r="M65" s="23"/>
       <c r="N65" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O65" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P65" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q65" s="24"/>
       <c r="R65" s="11"/>
@@ -5414,20 +5375,20 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="E66" s="23"/>
       <c r="F66" s="24" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
       <c r="G66" s="52"/>
       <c r="H66" s="24"/>
@@ -5437,13 +5398,13 @@
       <c r="L66" s="24"/>
       <c r="M66" s="23"/>
       <c r="N66" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O66" s="24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P66" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q66" s="24"/>
       <c r="R66" s="11"/>
@@ -5451,18 +5412,18 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
-        <v>268</v>
+        <v>521</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="C67" s="34"/>
       <c r="D67" s="34" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="E67" s="34"/>
       <c r="F67" s="35" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="G67" s="53"/>
       <c r="H67" s="35"/>
@@ -5472,13 +5433,13 @@
       <c r="L67" s="35"/>
       <c r="M67" s="34"/>
       <c r="N67" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O67" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P67" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q67" s="35"/>
       <c r="R67" s="11"/>
@@ -5486,20 +5447,20 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
-        <v>272</v>
+        <v>522</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="E68" s="34"/>
       <c r="F68" s="35" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="G68" s="53"/>
       <c r="H68" s="35"/>
@@ -5509,13 +5470,13 @@
       <c r="L68" s="35"/>
       <c r="M68" s="34"/>
       <c r="N68" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O68" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P68" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q68" s="35"/>
       <c r="R68" s="11"/>
@@ -5523,20 +5484,20 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>276</v>
+        <v>523</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="C69" s="34" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="E69" s="34"/>
       <c r="F69" s="35" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="G69" s="53"/>
       <c r="H69" s="35"/>
@@ -5546,114 +5507,114 @@
       <c r="L69" s="35"/>
       <c r="M69" s="34"/>
       <c r="N69" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O69" s="35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P69" s="35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q69" s="35"/>
       <c r="R69" s="11"/>
       <c r="S69" s="77"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
-        <v>279</v>
+      <c r="A70" s="16">
+        <v>40</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>280</v>
+        <v>239</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
       <c r="E70" s="17"/>
       <c r="F70" s="18" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
       <c r="G70" s="88" t="s">
-        <v>519</v>
+        <v>476</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="I70" s="66" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J70" s="20">
         <v>7</v>
       </c>
       <c r="K70" s="103" t="s">
-        <v>522</v>
+        <v>479</v>
       </c>
       <c r="L70" s="18"/>
       <c r="M70" s="103" t="s">
-        <v>525</v>
+        <v>482</v>
       </c>
       <c r="N70" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O70" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P70" s="18" t="s">
         <v>10</v>
-      </c>
-      <c r="O70" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="P70" s="18" t="s">
-        <v>12</v>
       </c>
       <c r="Q70" s="18"/>
       <c r="R70" s="11"/>
       <c r="S70" s="77" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A71" s="38" t="s">
-        <v>283</v>
+      <c r="A71" s="38">
+        <v>41</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>284</v>
+        <v>242</v>
       </c>
       <c r="C71" s="39"/>
       <c r="D71" s="39" t="s">
-        <v>380</v>
+        <v>337</v>
       </c>
       <c r="E71" s="39"/>
       <c r="F71" s="40" t="s">
-        <v>285</v>
+        <v>243</v>
       </c>
       <c r="G71" s="104" t="s">
-        <v>520</v>
+        <v>477</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="I71" s="73" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="J71" s="42">
         <v>63</v>
       </c>
       <c r="K71" s="106" t="s">
-        <v>523</v>
+        <v>480</v>
       </c>
       <c r="L71" s="40"/>
       <c r="M71" s="39"/>
       <c r="N71" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="O71" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="P71" s="40" t="s">
         <v>10</v>
-      </c>
-      <c r="O71" s="40" t="s">
-        <v>286</v>
-      </c>
-      <c r="P71" s="40" t="s">
-        <v>12</v>
       </c>
       <c r="Q71" s="40"/>
       <c r="R71" s="11"/>
       <c r="S71" s="77" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -5661,52 +5622,52 @@
         <v>42</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>288</v>
+        <v>246</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
       <c r="G72" s="105" t="s">
-        <v>521</v>
+        <v>478</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="I72" s="66" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="J72" s="20">
         <v>4</v>
       </c>
       <c r="K72" s="107" t="s">
-        <v>524</v>
+        <v>481</v>
       </c>
       <c r="L72" s="18"/>
       <c r="M72" s="17"/>
       <c r="N72" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O72" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P72" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="O72" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="P72" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="Q72" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R72" s="11"/>
       <c r="S72" s="77" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>